<commit_message>
under working for used material
</commit_message>
<xml_diff>
--- a/Nado Game/pyqt5/자재관리/widget_table.xlsx
+++ b/Nado Game/pyqt5/자재관리/widget_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\source\pygame\Nado Game\pyqt5\자재관리\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\pygame\Nado Game\pyqt5\자재관리\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02B9FB5-B4E5-497B-8933-9EAEBF7329FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDA3B52-A4A4-4498-B0E4-160C2711B3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="1155" windowWidth="18990" windowHeight="14280" xr2:uid="{33746BDE-84F1-4B14-B48D-C80B15739E68}"/>
+    <workbookView xWindow="43830" yWindow="1725" windowWidth="12075" windowHeight="13230" xr2:uid="{33746BDE-84F1-4B14-B48D-C80B15739E68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -340,7 +340,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -363,13 +363,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -378,6 +415,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,21 +742,21 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.69921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5" customWidth="1"/>
-    <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,8 +776,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -740,7 +786,7 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -750,15 +796,15 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="4"/>
       <c r="F3" s="2" t="s">
         <v>55</v>
       </c>
@@ -766,79 +812,79 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="2" t="s">
         <v>57</v>
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="2"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="2"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="5"/>
       <c r="F8" s="2"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>58</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -848,15 +894,15 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="2" t="s">
         <v>60</v>
       </c>
@@ -864,15 +910,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="2" t="s">
         <v>62</v>
       </c>
@@ -880,15 +926,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="2" t="s">
         <v>55</v>
       </c>
@@ -896,65 +942,65 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="2"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="2"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16" s="4"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="2"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A17" s="4"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="5"/>
       <c r="F17" s="2"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A18" s="5"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="3" t="s">
         <v>65</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -964,8 +1010,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -974,7 +1020,7 @@
       <c r="C19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="4"/>
       <c r="F19" s="2" t="s">
         <v>60</v>
       </c>
@@ -982,15 +1028,15 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="4"/>
       <c r="F20" s="2" t="s">
         <v>62</v>
       </c>
@@ -998,15 +1044,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="4"/>
       <c r="F21" s="2" t="s">
         <v>55</v>
       </c>
@@ -1014,58 +1060,58 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="4"/>
       <c r="F22" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="4"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="1"/>
+      <c r="E24" s="4"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="5"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
         <v>46</v>
       </c>
@@ -1073,8 +1119,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
         <v>16</v>
       </c>
@@ -1082,8 +1128,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
         <v>49</v>
       </c>
@@ -1091,8 +1137,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
         <v>18</v>
       </c>
@@ -1100,24 +1146,31 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A30" s="4"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A31" s="4"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A32" s="5"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="A19:A32"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="E9:E17"/>
+    <mergeCell ref="E18:E25"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>